<commit_message>
Changed variable names for report
</commit_message>
<xml_diff>
--- a/Full ISA/Revised XM23 Instruction Set.xlsx
+++ b/Full ISA/Revised XM23 Instruction Set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27230b06e512bdd1/Courses/XMX-23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romes\OneDrive\Desktop\XM23-CPU\Full ISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{C76AF7B5-6ACC-4F56-B9C4-C17BABEA1CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8E17D51-8EA7-4076-BC47-A03906F1E808}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475B2E45-56D9-404F-ABD2-5F6624A9E1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5DE55672-C90B-4D84-A3F4-2A7845A0AE44}"/>
+    <workbookView xWindow="-33017" yWindow="-4843" windowWidth="33120" windowHeight="18000" xr2:uid="{5DE55672-C90B-4D84-A3F4-2A7845A0AE44}"/>
   </bookViews>
   <sheets>
     <sheet name="XM3-23 (2)" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -549,12 +549,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,18 +572,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -627,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -733,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -875,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -885,9 +871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4B0825-EE94-4CA4-9DC2-1EA8BF9FE880}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,28 +2207,28 @@
       <c r="I24" s="12">
         <v>1</v>
       </c>
-      <c r="J24" s="22">
-        <v>0</v>
-      </c>
-      <c r="K24" s="22" t="s">
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="N24" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P24" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q24" s="23" t="s">
+      <c r="N24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q24" s="6" t="s">
         <v>53</v>
       </c>
       <c r="R24" s="7" t="s">
@@ -2277,28 +2263,28 @@
       <c r="I25" s="12">
         <v>0</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="22">
-        <v>0</v>
-      </c>
-      <c r="L25" s="22">
-        <v>0</v>
-      </c>
-      <c r="M25" s="23">
-        <v>0</v>
-      </c>
-      <c r="N25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q25" s="23" t="s">
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0</v>
+      </c>
+      <c r="M25" s="6">
+        <v>0</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" s="6" t="s">
         <v>55</v>
       </c>
       <c r="R25" s="7" t="s">
@@ -2333,28 +2319,28 @@
       <c r="I26" s="12">
         <v>0</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K26" s="22">
-        <v>0</v>
-      </c>
-      <c r="L26" s="22">
-        <v>0</v>
-      </c>
-      <c r="M26" s="23">
-        <v>1</v>
-      </c>
-      <c r="N26" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P26" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q26" s="23" t="s">
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0</v>
+      </c>
+      <c r="M26" s="6">
+        <v>1</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q26" s="6" t="s">
         <v>57</v>
       </c>
       <c r="R26" s="7" t="s">
@@ -2389,28 +2375,28 @@
       <c r="I27" s="12">
         <v>0</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K27" s="22">
-        <v>0</v>
-      </c>
-      <c r="L27" s="22">
-        <v>1</v>
-      </c>
-      <c r="M27" s="23">
-        <v>0</v>
-      </c>
-      <c r="N27" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O27" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P27" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q27" s="23" t="s">
+      <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <v>1</v>
+      </c>
+      <c r="M27" s="6">
+        <v>0</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" s="6" t="s">
         <v>59</v>
       </c>
       <c r="R27" s="7" t="s">
@@ -2445,28 +2431,28 @@
       <c r="I28" s="12">
         <v>0</v>
       </c>
-      <c r="J28" s="22">
-        <v>0</v>
-      </c>
-      <c r="K28" s="22">
-        <v>0</v>
-      </c>
-      <c r="L28" s="22">
-        <v>1</v>
-      </c>
-      <c r="M28" s="23">
-        <v>1</v>
-      </c>
-      <c r="N28" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O28" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P28" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q28" s="23" t="s">
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0</v>
+      </c>
+      <c r="L28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28" s="6">
+        <v>1</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q28" s="6" t="s">
         <v>61</v>
       </c>
       <c r="R28" s="7" t="s">
@@ -2501,28 +2487,28 @@
       <c r="I29" s="12">
         <v>0</v>
       </c>
-      <c r="J29" s="22">
-        <v>0</v>
-      </c>
-      <c r="K29" s="22">
-        <v>1</v>
-      </c>
-      <c r="L29" s="22">
-        <v>0</v>
-      </c>
-      <c r="M29" s="23">
-        <v>0</v>
-      </c>
-      <c r="N29" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O29" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P29" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q29" s="23" t="s">
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
+        <v>1</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="M29" s="6">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q29" s="6" t="s">
         <v>63</v>
       </c>
       <c r="R29" s="7" t="s">
@@ -2557,28 +2543,28 @@
       <c r="I30" s="12">
         <v>1</v>
       </c>
-      <c r="J30" s="22">
-        <v>0</v>
-      </c>
-      <c r="K30" s="22">
-        <v>0</v>
-      </c>
-      <c r="L30" s="22">
-        <v>0</v>
-      </c>
-      <c r="M30" s="23">
-        <v>0</v>
-      </c>
-      <c r="N30" s="22" t="s">
+      <c r="J30" s="5">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5">
+        <v>0</v>
+      </c>
+      <c r="M30" s="6">
+        <v>0</v>
+      </c>
+      <c r="N30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="O30" s="22" t="s">
+      <c r="O30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="P30" s="22" t="s">
+      <c r="P30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q30" s="23" t="s">
+      <c r="Q30" s="6" t="s">
         <v>66</v>
       </c>
       <c r="R30" s="7" t="s">
@@ -2613,28 +2599,28 @@
       <c r="I31" s="12">
         <v>1</v>
       </c>
-      <c r="J31" s="22">
-        <v>0</v>
-      </c>
-      <c r="K31" s="22">
-        <v>0</v>
-      </c>
-      <c r="L31" s="22">
-        <v>1</v>
-      </c>
-      <c r="M31" s="23" t="s">
+      <c r="J31" s="5">
+        <v>0</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0</v>
+      </c>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N31" s="22" t="s">
+      <c r="N31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="O31" s="22" t="s">
+      <c r="O31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P31" s="22" t="s">
+      <c r="P31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Q31" s="23" t="s">
+      <c r="Q31" s="6" t="s">
         <v>69</v>
       </c>
       <c r="R31" s="7" t="s">
@@ -2669,28 +2655,28 @@
       <c r="I32" s="12">
         <v>1</v>
       </c>
-      <c r="J32" s="22">
-        <v>0</v>
-      </c>
-      <c r="K32" s="22">
-        <v>1</v>
-      </c>
-      <c r="L32" s="22" t="s">
+      <c r="J32" s="5">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5">
+        <v>1</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="M32" s="23" t="s">
+      <c r="M32" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="N32" s="22" t="s">
+      <c r="N32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O32" s="22" t="s">
+      <c r="O32" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="P32" s="22" t="s">
+      <c r="P32" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Q32" s="23" t="s">
+      <c r="Q32" s="6" t="s">
         <v>76</v>
       </c>
       <c r="R32" s="7" t="s">
@@ -2725,28 +2711,28 @@
       <c r="I33" s="12">
         <v>1</v>
       </c>
-      <c r="J33" s="22">
-        <v>1</v>
-      </c>
-      <c r="K33" s="22">
-        <v>0</v>
-      </c>
-      <c r="L33" s="22" t="s">
+      <c r="J33" s="5">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5">
+        <v>0</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="M33" s="23" t="s">
+      <c r="M33" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="N33" s="22" t="s">
+      <c r="N33" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O33" s="22" t="s">
+      <c r="O33" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="P33" s="22" t="s">
+      <c r="P33" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Q33" s="23" t="s">
+      <c r="Q33" s="6" t="s">
         <v>78</v>
       </c>
       <c r="R33" s="7" t="s">
@@ -2922,19 +2908,19 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="24">
-        <v>0</v>
-      </c>
-      <c r="B37" s="24">
-        <v>1</v>
-      </c>
-      <c r="C37" s="24">
-        <v>1</v>
-      </c>
-      <c r="D37" s="24">
-        <v>0</v>
-      </c>
-      <c r="E37" s="25">
+      <c r="A37" s="22">
+        <v>0</v>
+      </c>
+      <c r="B37" s="22">
+        <v>1</v>
+      </c>
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
+      <c r="D37" s="22">
+        <v>0</v>
+      </c>
+      <c r="E37" s="23">
         <v>0</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -2978,19 +2964,19 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="24">
-        <v>0</v>
-      </c>
-      <c r="B38" s="24">
-        <v>1</v>
-      </c>
-      <c r="C38" s="24">
-        <v>1</v>
-      </c>
-      <c r="D38" s="24">
-        <v>0</v>
-      </c>
-      <c r="E38" s="25">
+      <c r="A38" s="22">
+        <v>0</v>
+      </c>
+      <c r="B38" s="22">
+        <v>1</v>
+      </c>
+      <c r="C38" s="22">
+        <v>1</v>
+      </c>
+      <c r="D38" s="22">
+        <v>0</v>
+      </c>
+      <c r="E38" s="23">
         <v>1</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -3034,19 +3020,19 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="24">
-        <v>0</v>
-      </c>
-      <c r="B39" s="24">
-        <v>1</v>
-      </c>
-      <c r="C39" s="24">
-        <v>1</v>
-      </c>
-      <c r="D39" s="24">
-        <v>1</v>
-      </c>
-      <c r="E39" s="25">
+      <c r="A39" s="22">
+        <v>0</v>
+      </c>
+      <c r="B39" s="22">
+        <v>1</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1</v>
+      </c>
+      <c r="D39" s="22">
+        <v>1</v>
+      </c>
+      <c r="E39" s="23">
         <v>0</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -3090,19 +3076,19 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="24">
-        <v>0</v>
-      </c>
-      <c r="B40" s="24">
-        <v>1</v>
-      </c>
-      <c r="C40" s="24">
-        <v>1</v>
-      </c>
-      <c r="D40" s="24">
-        <v>1</v>
-      </c>
-      <c r="E40" s="25">
+      <c r="A40" s="22">
+        <v>0</v>
+      </c>
+      <c r="B40" s="22">
+        <v>1</v>
+      </c>
+      <c r="C40" s="22">
+        <v>1</v>
+      </c>
+      <c r="D40" s="22">
+        <v>1</v>
+      </c>
+      <c r="E40" s="23">
         <v>1</v>
       </c>
       <c r="F40" s="5" t="s">

</xml_diff>